<commit_message>
added better recomendation list
</commit_message>
<xml_diff>
--- a/docs/DTT-Assessment-Hour-Log.xlsx
+++ b/docs/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktorharhat/Documents/rogram/uni/DTT-Frontend-Assignment/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE41151-E224-1148-BC23-02AAC2204D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3FEAF5-B556-944F-99BC-A0444C098852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="840" windowWidth="29920" windowHeight="18640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Subject</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t xml:space="preserve">For delete modal when screen where below 640px I changed it width to take more space on screen and put button to column. The about page was easy, as I just needed to add correct font sizing for mobile. </t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Made recommendation list to be displayed by three criterias</t>
+  </si>
+  <si>
+    <t>I decided to make recommendation list more accurate, I choosed price, size and location. I created simularity score function that is executed to each house in recomndation list, and adds simularity score to each house by comparing house on current page and all other houses. The simularity score (1-0) is calculated by formula that takes current and other houses prices or sizes and finds how close they are relative to the largest price between two of them, where 1 means identical prices and 0 means maximum difference. Than it sorts houses by that score filed and takes first three asuming they are most simular to current house.</t>
   </si>
 </sst>
 </file>
@@ -527,7 +536,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -573,9 +582,6 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -584,6 +590,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -596,9 +605,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1860,7 +1866,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1916,13 +1922,13 @@
       <c r="B4" s="22">
         <v>0.5</v>
       </c>
-      <c r="C4" s="23">
-        <v>45997</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="18">
+        <v>45820</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.2">
@@ -1932,13 +1938,13 @@
       <c r="B5" s="22">
         <v>0.5</v>
       </c>
-      <c r="C5" s="23">
-        <v>45997</v>
-      </c>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="18">
+        <v>45820</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
@@ -1949,12 +1955,12 @@
         <v>1</v>
       </c>
       <c r="C6" s="18">
-        <v>45997</v>
+        <v>45820</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.2">
@@ -1965,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="18">
-        <v>45997</v>
+        <v>45820</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>27</v>
@@ -1981,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="18">
-        <v>45997</v>
+        <v>45820</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>28</v>
@@ -1997,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="18">
-        <v>45997</v>
+        <v>45820</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>29</v>
@@ -2013,7 +2019,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="18">
-        <v>45997</v>
+        <v>45820</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>30</v>
@@ -2029,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="18">
-        <v>45997</v>
+        <v>45821</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>31</v>
@@ -2045,7 +2051,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="18">
-        <v>45998</v>
+        <v>45821</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>32</v>
@@ -2061,9 +2067,9 @@
         <v>2</v>
       </c>
       <c r="C13" s="18">
-        <v>45998</v>
-      </c>
-      <c r="D13" s="31" t="s">
+        <v>45821</v>
+      </c>
+      <c r="D13" s="26" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="19"/>
@@ -2077,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="18">
-        <v>45998</v>
+        <v>45821</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>34</v>
@@ -2093,12 +2099,12 @@
         <v>1</v>
       </c>
       <c r="C15" s="18">
-        <v>45998</v>
+        <v>45821</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="25" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="4"/>
@@ -2111,12 +2117,12 @@
         <v>1</v>
       </c>
       <c r="C16" s="18">
-        <v>45998</v>
+        <v>45821</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="26"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -2127,7 +2133,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="18">
-        <v>45998</v>
+        <v>45821</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>37</v>
@@ -2143,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="18">
-        <v>45998</v>
+        <v>45821</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>38</v>
@@ -2159,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="18">
-        <v>45998</v>
+        <v>45821</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>39</v>
@@ -2167,12 +2173,22 @@
       <c r="E19" s="19"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="26"/>
+    <row r="20" spans="1:6" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="17">
+        <v>1</v>
+      </c>
+      <c r="C20" s="18">
+        <v>45822</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>